<commit_message>
added sheets and changed names
</commit_message>
<xml_diff>
--- a/experiments/experiment_template.xlsx
+++ b/experiments/experiment_template.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C42192-C35A-3442-A87E-6648C2873AEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F10987E-8919-D443-8959-236A1FDE45A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="-20840" windowWidth="25440" windowHeight="14540" activeTab="1" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="11840" yWindow="-19300" windowWidth="25440" windowHeight="14540" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
-    <sheet name="Description" sheetId="2" r:id="rId1"/>
-    <sheet name="Specification" sheetId="1" r:id="rId2"/>
+    <sheet name="experiment-description" sheetId="2" r:id="rId1"/>
+    <sheet name="experiment-specification" sheetId="1" r:id="rId2"/>
+    <sheet name="run-description" sheetId="4" r:id="rId3"/>
+    <sheet name="run-specification" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,9 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
-  <si>
-    <t>id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+  <si>
+    <t>experiment_id</t>
   </si>
   <si>
     <t>name</t>
@@ -92,6 +94,15 @@
   </si>
   <si>
     <t>extended</t>
+  </si>
+  <si>
+    <t>run_id</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Dummy</t>
   </si>
 </sst>
 </file>
@@ -446,11 +457,12 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
   </cols>
@@ -497,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914169FE-D361-6946-A1DD-9152CD547001}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,4 +654,75 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A476CE8A-A8FA-4046-81E7-5C8AA6B64C8D}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new experiment R file and changes to experiment xslx file. Coding file changed as well
</commit_message>
<xml_diff>
--- a/experiments/experiment_template.xlsx
+++ b/experiments/experiment_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjs/projects/covid/BCS/experiments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solviro/Documents/COVID-19/BCS/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F10987E-8919-D443-8959-236A1FDE45A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54E8938-FEE7-4C41-9854-5310FCD32194}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11840" yWindow="-19300" windowWidth="25440" windowHeight="14540" activeTab="3" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{2B698B52-4F40-4A42-8D71-F94349FB2461}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment-description" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>experiment_id</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>base</t>
-  </si>
-  <si>
-    <t>extended</t>
   </si>
   <si>
     <t>run_id</t>
@@ -454,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C70F787-7AA1-8E4F-AD58-B726756111FE}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,11 +490,6 @@
       </c>
       <c r="D2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -668,7 +660,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -682,10 +674,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -697,7 +689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A112CAC-8916-A049-B0DC-1F9A9140A276}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -708,7 +700,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>

</xml_diff>